<commit_message>
feat: new dummyData structure incl. samples for put, get and delete from an to firebase
</commit_message>
<xml_diff>
--- a/design/Join_Projektuebersicht.xlsx
+++ b/design/Join_Projektuebersicht.xlsx
@@ -59,26 +59,7 @@
     <t>Datei (HTML)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Einstieg; z. B. Landing oder Redirect zu </t>
-    </r>
-    <r>
-      <rPr>
-        <color theme="1"/>
-        <sz val="10"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>pages/login.html</t>
-    </r>
-    <r>
-      <rPr>
-        <color theme="1"/>
-        <family val="2"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> oder Summary.youtube​</t>
-    </r>
+    <t>Einstieg; z. B. Landing oder Redirect zu pages/login.html oder Summary.youtube​</t>
   </si>
   <si>
     <t>pages/</t>

</xml_diff>